<commit_message>
QuickStart now skip lobby / make quick test a bit easy
</commit_message>
<xml_diff>
--- a/read me.xlsx
+++ b/read me.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main\Code\Unity\comp-3770-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268AFB24-1C40-4832-B424-8DFC5D539B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A155A7-2F9A-4045-BF4C-B126E10D56C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3645" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2ADC3FCF-CCF9-49D6-B6E7-A871AFAD5DC6}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{2ADC3FCF-CCF9-49D6-B6E7-A871AFAD5DC6}"/>
   </bookViews>
   <sheets>
-    <sheet name="NavMesh" sheetId="1" r:id="rId1"/>
-    <sheet name="Lobby" sheetId="2" r:id="rId2"/>
-    <sheet name="Map teleport" sheetId="3" r:id="rId3"/>
+    <sheet name="Howto Spawn Player" sheetId="4" r:id="rId1"/>
+    <sheet name="NavMesh" sheetId="1" r:id="rId2"/>
+    <sheet name="Lobby" sheetId="2" r:id="rId3"/>
+    <sheet name="Map teleport" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1683,6 +1684,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8793909-30B0-4433-A1E6-944255CB4131}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DBAE8A-B62B-44B8-9E77-443E29760446}">
   <dimension ref="A1:E105"/>
   <sheetViews>
@@ -1785,7 +1801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972D0697-1635-4141-8371-FBF7C7C1C9AF}">
   <dimension ref="A1:D102"/>
   <sheetViews>
@@ -1890,12 +1906,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F66297B5-D8AD-4A9D-ACD5-58CB0E507482}">
   <dimension ref="B3:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.149999999999999"/>

</xml_diff>